<commit_message>
Something to show your supervisor
</commit_message>
<xml_diff>
--- a/Data/QUESTION_MOCK.xlsx
+++ b/Data/QUESTION_MOCK.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ARINZE PC\Documents\Masters Project\Career Advice System\Back-End\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ARINZE PC\Documents\Alfred\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE1E3A21-B7FD-4FD1-92A1-FB125CEF7DB4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF1CD727-243F-4B52-8058-E52F10B8A4EB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
   <si>
     <t>question</t>
   </si>
@@ -28,13 +28,16 @@
     <t>type</t>
   </si>
   <si>
-    <t>Can you play a musical instrument?</t>
-  </si>
-  <si>
-    <t>artistic</t>
-  </si>
-  <si>
-    <t>Can you dance?</t>
+    <t>Engineering</t>
+  </si>
+  <si>
+    <t>Have you ever been to a work shop?</t>
+  </si>
+  <si>
+    <t>Have you used auto card before?</t>
+  </si>
+  <si>
+    <t>Have u fixed a tire before</t>
   </si>
 </sst>
 </file>
@@ -384,10 +387,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -413,10 +416,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
         <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -424,7 +427,15 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>